<commit_message>
MissionSystem, Data, Component 추가(수정), 팝업 추가 등 UI 대응,, 근데 팝업이 안뜸
</commit_message>
<xml_diff>
--- a/Design/Excels/StringTable.xlsx
+++ b/Design/Excels/StringTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JH\UnityProjects\BeautifulDeathMatch\Beautiful-DeathMatch\Design\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FAE4A1-8F72-489F-8422-0B00A19C1DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428E56B1-6A21-4534-A204-5E3056B10497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2016" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2424" yWindow="1896" windowWidth="23064" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="StringKey" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>string</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -135,6 +135,112 @@
   </si>
   <si>
     <t>en8</t>
+  </si>
+  <si>
+    <t>sys.hud.interaction.mission</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F를 눌러 미션 시작: {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>en9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys.mission.name.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys.mission.name.2</t>
+  </si>
+  <si>
+    <t>sys.mission.name.3</t>
+  </si>
+  <si>
+    <t>sys.mission.name.4</t>
+  </si>
+  <si>
+    <t>sys.mission.name.5</t>
+  </si>
+  <si>
+    <t>sys.mission.content.1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys.mission.content.2</t>
+  </si>
+  <si>
+    <t>sys.mission.content.3</t>
+  </si>
+  <si>
+    <t>sys.mission.content.4</t>
+  </si>
+  <si>
+    <t>sys.mission.content.5</t>
+  </si>
+  <si>
+    <t>미션 1 이름입니다~~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미션 2 이름입니다~~</t>
+  </si>
+  <si>
+    <t>미션 3 이름입니다~~</t>
+  </si>
+  <si>
+    <t>미션 4 이름입니다~~</t>
+  </si>
+  <si>
+    <t>미션 5 이름입니다~~</t>
+  </si>
+  <si>
+    <t>미션 1 내용입니다~~ 임시로 넣어놓은 긴 내용입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미션 2 내용입니다~~ 임시로 넣어놓은 긴 내용입니다.</t>
+  </si>
+  <si>
+    <t>미션 3 내용입니다~~ 임시로 넣어놓은 긴 내용입니다.</t>
+  </si>
+  <si>
+    <t>미션 4 내용입니다~~ 임시로 넣어놓은 긴 내용입니다.</t>
+  </si>
+  <si>
+    <t>미션 5 내용입니다~~ 임시로 넣어놓은 긴 내용입니다.</t>
+  </si>
+  <si>
+    <t>en10</t>
+  </si>
+  <si>
+    <t>en11</t>
+  </si>
+  <si>
+    <t>en12</t>
+  </si>
+  <si>
+    <t>en13</t>
+  </si>
+  <si>
+    <t>en14</t>
+  </si>
+  <si>
+    <t>en15</t>
+  </si>
+  <si>
+    <t>en16</t>
+  </si>
+  <si>
+    <t>en17</t>
+  </si>
+  <si>
+    <t>en18</t>
+  </si>
+  <si>
+    <t>en19</t>
   </si>
 </sst>
 </file>
@@ -459,7 +565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E390BA2F-98DF-4E9B-B8EA-7EEE2DEF3255}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,6 +686,127 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>